<commit_message>
verwerken van EKS-proces in Blik
</commit_message>
<xml_diff>
--- a/Blik/Medewerkers.xlsx
+++ b/Blik/Medewerkers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="210" windowWidth="15195" windowHeight="8325" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="270" windowWidth="15195" windowHeight="8265" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="medewerkers" sheetId="5" r:id="rId1"/>
@@ -1028,7 +1028,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1180,6 +1180,13 @@
       <b/>
       <sz val="8"/>
       <name val="Agrofont"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1519,7 +1526,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1557,6 +1564,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="21" fillId="24" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -78836,7 +78846,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" thickBot="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="19" t="s">
         <v>327</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -79580,7 +79590,7 @@
       <c r="A167"/>
       <c r="B167"/>
     </row>
-    <row r="169" spans="1:2"/>
+    <row r="169" spans="1:2" ht="12.75"/>
     <row r="170" spans="1:2" ht="12.75"/>
     <row r="171" spans="1:2" ht="12.75"/>
     <row r="172" spans="1:2" ht="12.75"/>

</xml_diff>

<commit_message>
Data analysis in Blik
</commit_message>
<xml_diff>
--- a/Blik/Medewerkers.xlsx
+++ b/Blik/Medewerkers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="270" windowWidth="15195" windowHeight="8265" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="330" windowWidth="15195" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="medewerkers" sheetId="5" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Dienstverbanden" sheetId="9" r:id="rId3"/>
     <sheet name="WTR" sheetId="10" r:id="rId4"/>
     <sheet name="Teams" sheetId="11" r:id="rId5"/>
-    <sheet name="Divisies" sheetId="12" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">medewerkers!#REF!</definedName>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10106" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10073" uniqueCount="328">
   <si>
     <t>Dhr. A. BAAS</t>
   </si>
@@ -985,9 +984,6 @@
     <t>Divisie Landbouw en Natuur</t>
   </si>
   <si>
-    <t>NVWA</t>
-  </si>
-  <si>
     <t>RO</t>
   </si>
   <si>
@@ -1003,12 +999,6 @@
     <t>Divisie Veterinair en Import</t>
   </si>
   <si>
-    <t>divisienaam</t>
-  </si>
-  <si>
-    <t>[Divisie]</t>
-  </si>
-  <si>
     <t>Divisie Inlichtingen en Opsporingsdienst</t>
   </si>
   <si>
@@ -1017,18 +1007,12 @@
   <si>
     <t>Bureau Risicobeoord en Onderzoeksprogrammering</t>
   </si>
-  <si>
-    <t>eenheidnr</t>
-  </si>
-  <si>
-    <t>Nederlandse Voedsel- en Warenautoriteit</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1182,13 +1166,6 @@
       <name val="Agrofont"/>
       <family val="2"/>
     </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="25">
     <fill>
@@ -1314,7 +1291,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1470,17 +1447,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="22"/>
-      </left>
-      <right style="medium">
-        <color indexed="22"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1526,7 +1492,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1562,13 +1528,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="24" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1913,9 +1872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -77661,7 +77618,7 @@
         <v>316</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="64" spans="1:4" thickBot="1">
@@ -77774,7 +77731,7 @@
         <v>317</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="74" spans="1:4" thickBot="1">
@@ -78316,10 +78273,10 @@
         <v>38</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="123" spans="1:4" thickBot="1">
@@ -78330,7 +78287,7 @@
         <v>38</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="124" spans="1:4" thickBot="1">
@@ -78341,7 +78298,7 @@
         <v>38</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="125" spans="1:4" thickBot="1">
@@ -78352,7 +78309,7 @@
         <v>38</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="126" spans="1:4" thickBot="1">
@@ -78363,10 +78320,10 @@
         <v>39</v>
       </c>
       <c r="C126" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="D126" s="8" t="s">
         <v>322</v>
-      </c>
-      <c r="D126" s="8" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="127" spans="1:4" thickBot="1">
@@ -78377,7 +78334,7 @@
         <v>39</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="128" spans="1:4" thickBot="1">
@@ -78388,7 +78345,7 @@
         <v>39</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="129" spans="1:4" thickBot="1">
@@ -78399,7 +78356,7 @@
         <v>39</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="130" spans="1:4" thickBot="1">
@@ -78410,7 +78367,7 @@
         <v>39</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="131" spans="1:4" thickBot="1">
@@ -78421,7 +78378,7 @@
         <v>39</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="132" spans="1:4" thickBot="1">
@@ -78432,7 +78389,7 @@
         <v>39</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="133" spans="1:4" thickBot="1">
@@ -78443,7 +78400,7 @@
         <v>39</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="134" spans="1:4" thickBot="1">
@@ -78454,10 +78411,10 @@
         <v>19</v>
       </c>
       <c r="C134" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="D134" s="8" t="s">
         <v>324</v>
-      </c>
-      <c r="D134" s="8" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="135" spans="1:4" thickBot="1">
@@ -78468,7 +78425,7 @@
         <v>19</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="136" spans="1:4" thickBot="1">
@@ -78479,7 +78436,7 @@
         <v>19</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="137" spans="1:4" thickBot="1">
@@ -78490,7 +78447,7 @@
         <v>19</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="138" spans="1:4" thickBot="1">
@@ -78501,7 +78458,7 @@
         <v>19</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="139" spans="1:4" thickBot="1">
@@ -78512,7 +78469,7 @@
         <v>19</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="140" spans="1:4" thickBot="1">
@@ -78523,7 +78480,7 @@
         <v>19</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="141" spans="1:4" thickBot="1">
@@ -78534,7 +78491,7 @@
         <v>19</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="142" spans="1:4" thickBot="1">
@@ -78545,7 +78502,7 @@
         <v>19</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="143" spans="1:4" thickBot="1">
@@ -78556,7 +78513,7 @@
         <v>19</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="144" spans="1:4" thickBot="1">
@@ -78567,7 +78524,7 @@
         <v>19</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="145" spans="1:3" thickBot="1">
@@ -78578,7 +78535,7 @@
         <v>19</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="146" spans="1:3" thickBot="1">
@@ -78589,7 +78546,7 @@
         <v>19</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="147" spans="1:3" thickBot="1">
@@ -78600,7 +78557,7 @@
         <v>19</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="148" spans="1:3" thickBot="1">
@@ -78611,7 +78568,7 @@
         <v>19</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="149" spans="1:3" thickBot="1">
@@ -78622,7 +78579,7 @@
         <v>19</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="150" spans="1:3" thickBot="1">
@@ -78633,7 +78590,7 @@
         <v>19</v>
       </c>
       <c r="C150" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="151" spans="1:3" thickBot="1">
@@ -78644,7 +78601,7 @@
         <v>19</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="152" spans="1:3" thickBot="1">
@@ -78655,7 +78612,7 @@
         <v>19</v>
       </c>
       <c r="C152" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="153" spans="1:3" thickBot="1">
@@ -78666,7 +78623,7 @@
         <v>19</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="154" spans="1:3" thickBot="1">
@@ -78677,7 +78634,7 @@
         <v>19</v>
       </c>
       <c r="C154" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="155" spans="1:3" thickBot="1">
@@ -78688,7 +78645,7 @@
         <v>19</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="156" spans="1:3" thickBot="1">
@@ -78699,7 +78656,7 @@
         <v>19</v>
       </c>
       <c r="C156" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="157" spans="1:3" thickBot="1">
@@ -78710,7 +78667,7 @@
         <v>19</v>
       </c>
       <c r="C157" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="158" spans="1:3" thickBot="1">
@@ -78721,7 +78678,7 @@
         <v>19</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="159" spans="1:3" thickBot="1">
@@ -78732,7 +78689,7 @@
         <v>19</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="160" spans="1:3" thickBot="1">
@@ -78743,7 +78700,7 @@
         <v>19</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="161" spans="1:3" thickBot="1">
@@ -78754,7 +78711,7 @@
         <v>19</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="162" spans="1:3" thickBot="1">
@@ -78765,7 +78722,7 @@
         <v>19</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="163" spans="1:3" thickBot="1">
@@ -78776,7 +78733,7 @@
         <v>19</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="164" spans="1:3" thickBot="1">
@@ -78787,7 +78744,7 @@
         <v>19</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="165" spans="1:3" thickBot="1">
@@ -78798,7 +78755,7 @@
         <v>19</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="166" spans="1:3" thickBot="1">
@@ -78809,7 +78766,7 @@
         <v>19</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="167" spans="1:3" thickBot="1">
@@ -78820,7 +78777,7 @@
         <v>19</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="12.75"/>
@@ -78831,770 +78788,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C172"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" thickBottom="1"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" style="8" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" thickBot="1">
-      <c r="A1" s="19" t="s">
-        <v>327</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" thickBot="1">
-      <c r="A2" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" thickBot="1">
-      <c r="A3" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" thickBot="1">
-      <c r="A4" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" thickBot="1">
-      <c r="A5" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" thickBot="1">
-      <c r="A6" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" thickBot="1">
-      <c r="A7" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" thickBot="1">
-      <c r="A8" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" thickBot="1">
-      <c r="A9" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" thickBot="1">
-      <c r="A10" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" thickBot="1">
-      <c r="A11" s="18" t="s">
-        <v>320</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>332</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="12.75">
-      <c r="A12"/>
-      <c r="B12"/>
-    </row>
-    <row r="13" spans="1:3" ht="12.75">
-      <c r="A13"/>
-      <c r="B13"/>
-    </row>
-    <row r="14" spans="1:3" ht="12.75">
-      <c r="A14"/>
-      <c r="B14"/>
-    </row>
-    <row r="15" spans="1:3" ht="12.75">
-      <c r="A15"/>
-      <c r="B15"/>
-    </row>
-    <row r="16" spans="1:3" ht="12.75">
-      <c r="A16"/>
-      <c r="B16"/>
-    </row>
-    <row r="17" spans="1:2" ht="12.75">
-      <c r="A17"/>
-      <c r="B17"/>
-    </row>
-    <row r="18" spans="1:2" ht="12.75">
-      <c r="A18"/>
-      <c r="B18"/>
-    </row>
-    <row r="19" spans="1:2" ht="12.75">
-      <c r="A19"/>
-      <c r="B19"/>
-    </row>
-    <row r="20" spans="1:2" ht="12.75">
-      <c r="A20"/>
-      <c r="B20"/>
-    </row>
-    <row r="21" spans="1:2" ht="12.75">
-      <c r="A21"/>
-      <c r="B21"/>
-    </row>
-    <row r="22" spans="1:2" ht="12.75">
-      <c r="A22"/>
-      <c r="B22"/>
-    </row>
-    <row r="23" spans="1:2" ht="12.75">
-      <c r="A23"/>
-      <c r="B23"/>
-    </row>
-    <row r="24" spans="1:2" ht="12.75">
-      <c r="A24"/>
-      <c r="B24"/>
-    </row>
-    <row r="25" spans="1:2" ht="12.75">
-      <c r="A25"/>
-      <c r="B25"/>
-    </row>
-    <row r="26" spans="1:2" ht="12.75">
-      <c r="A26"/>
-      <c r="B26"/>
-    </row>
-    <row r="27" spans="1:2" ht="12.75">
-      <c r="A27"/>
-      <c r="B27"/>
-    </row>
-    <row r="28" spans="1:2" ht="12.75">
-      <c r="A28"/>
-      <c r="B28"/>
-    </row>
-    <row r="29" spans="1:2" ht="12.75">
-      <c r="A29"/>
-      <c r="B29"/>
-    </row>
-    <row r="30" spans="1:2" ht="12.75">
-      <c r="A30"/>
-      <c r="B30"/>
-    </row>
-    <row r="31" spans="1:2" ht="12.75">
-      <c r="A31"/>
-      <c r="B31"/>
-    </row>
-    <row r="32" spans="1:2" ht="12.75">
-      <c r="A32"/>
-      <c r="B32"/>
-    </row>
-    <row r="33" spans="1:2" ht="12.75">
-      <c r="A33"/>
-      <c r="B33"/>
-    </row>
-    <row r="34" spans="1:2" ht="12.75">
-      <c r="A34"/>
-      <c r="B34"/>
-    </row>
-    <row r="35" spans="1:2" ht="12.75">
-      <c r="A35"/>
-      <c r="B35"/>
-    </row>
-    <row r="36" spans="1:2" ht="12.75">
-      <c r="A36"/>
-      <c r="B36"/>
-    </row>
-    <row r="37" spans="1:2" ht="12.75">
-      <c r="A37"/>
-      <c r="B37"/>
-    </row>
-    <row r="38" spans="1:2" ht="12.75">
-      <c r="A38"/>
-      <c r="B38"/>
-    </row>
-    <row r="39" spans="1:2" ht="12.75">
-      <c r="A39"/>
-      <c r="B39"/>
-    </row>
-    <row r="40" spans="1:2" ht="12.75">
-      <c r="A40"/>
-      <c r="B40"/>
-    </row>
-    <row r="41" spans="1:2" ht="12.75">
-      <c r="A41"/>
-      <c r="B41"/>
-    </row>
-    <row r="42" spans="1:2" ht="12.75">
-      <c r="A42"/>
-      <c r="B42"/>
-    </row>
-    <row r="43" spans="1:2" ht="12.75">
-      <c r="A43"/>
-      <c r="B43"/>
-    </row>
-    <row r="44" spans="1:2" ht="12.75">
-      <c r="A44"/>
-      <c r="B44"/>
-    </row>
-    <row r="45" spans="1:2" ht="12.75">
-      <c r="A45"/>
-      <c r="B45"/>
-    </row>
-    <row r="46" spans="1:2" ht="12.75">
-      <c r="A46"/>
-      <c r="B46"/>
-    </row>
-    <row r="47" spans="1:2" ht="12.75">
-      <c r="A47"/>
-      <c r="B47"/>
-    </row>
-    <row r="48" spans="1:2" ht="12.75">
-      <c r="A48"/>
-      <c r="B48"/>
-    </row>
-    <row r="49" spans="1:2" ht="12.75">
-      <c r="A49"/>
-      <c r="B49"/>
-    </row>
-    <row r="50" spans="1:2" ht="12.75">
-      <c r="A50"/>
-      <c r="B50"/>
-    </row>
-    <row r="51" spans="1:2" ht="12.75">
-      <c r="A51"/>
-      <c r="B51"/>
-    </row>
-    <row r="52" spans="1:2" ht="12.75">
-      <c r="A52"/>
-      <c r="B52"/>
-    </row>
-    <row r="53" spans="1:2" ht="12.75">
-      <c r="A53"/>
-      <c r="B53"/>
-    </row>
-    <row r="54" spans="1:2" ht="12.75">
-      <c r="A54"/>
-      <c r="B54"/>
-    </row>
-    <row r="55" spans="1:2" ht="12.75">
-      <c r="A55"/>
-      <c r="B55"/>
-    </row>
-    <row r="56" spans="1:2" ht="12.75">
-      <c r="A56"/>
-      <c r="B56"/>
-    </row>
-    <row r="57" spans="1:2" ht="12.75">
-      <c r="A57"/>
-      <c r="B57"/>
-    </row>
-    <row r="58" spans="1:2" ht="12.75">
-      <c r="A58"/>
-      <c r="B58"/>
-    </row>
-    <row r="59" spans="1:2" ht="12.75">
-      <c r="A59"/>
-      <c r="B59"/>
-    </row>
-    <row r="60" spans="1:2" ht="12.75">
-      <c r="A60"/>
-      <c r="B60"/>
-    </row>
-    <row r="61" spans="1:2" ht="12.75">
-      <c r="A61"/>
-      <c r="B61"/>
-    </row>
-    <row r="62" spans="1:2" ht="12.75">
-      <c r="A62"/>
-      <c r="B62"/>
-    </row>
-    <row r="63" spans="1:2" ht="12.75">
-      <c r="A63"/>
-      <c r="B63"/>
-    </row>
-    <row r="64" spans="1:2" ht="12.75">
-      <c r="A64"/>
-      <c r="B64"/>
-    </row>
-    <row r="65" spans="1:2" ht="12.75">
-      <c r="A65"/>
-      <c r="B65"/>
-    </row>
-    <row r="66" spans="1:2" ht="12.75">
-      <c r="A66"/>
-      <c r="B66"/>
-    </row>
-    <row r="67" spans="1:2" ht="12.75">
-      <c r="A67"/>
-      <c r="B67"/>
-    </row>
-    <row r="68" spans="1:2" ht="12.75">
-      <c r="A68"/>
-      <c r="B68"/>
-    </row>
-    <row r="69" spans="1:2" ht="12.75">
-      <c r="A69"/>
-      <c r="B69"/>
-    </row>
-    <row r="70" spans="1:2" ht="12.75">
-      <c r="A70"/>
-      <c r="B70"/>
-    </row>
-    <row r="71" spans="1:2" ht="12.75">
-      <c r="A71"/>
-      <c r="B71"/>
-    </row>
-    <row r="72" spans="1:2" ht="12.75">
-      <c r="A72"/>
-      <c r="B72"/>
-    </row>
-    <row r="73" spans="1:2" ht="12.75">
-      <c r="A73"/>
-      <c r="B73"/>
-    </row>
-    <row r="74" spans="1:2" ht="12.75">
-      <c r="A74"/>
-      <c r="B74"/>
-    </row>
-    <row r="75" spans="1:2" ht="12.75">
-      <c r="A75"/>
-      <c r="B75"/>
-    </row>
-    <row r="76" spans="1:2" ht="12.75">
-      <c r="A76"/>
-      <c r="B76"/>
-    </row>
-    <row r="77" spans="1:2" ht="12.75">
-      <c r="A77"/>
-      <c r="B77"/>
-    </row>
-    <row r="78" spans="1:2" ht="12.75">
-      <c r="A78"/>
-      <c r="B78"/>
-    </row>
-    <row r="79" spans="1:2" ht="12.75">
-      <c r="A79"/>
-      <c r="B79"/>
-    </row>
-    <row r="80" spans="1:2" ht="12.75">
-      <c r="A80"/>
-      <c r="B80"/>
-    </row>
-    <row r="81" spans="1:2" ht="12.75">
-      <c r="A81"/>
-      <c r="B81"/>
-    </row>
-    <row r="82" spans="1:2" ht="12.75">
-      <c r="A82"/>
-      <c r="B82"/>
-    </row>
-    <row r="83" spans="1:2" ht="12.75">
-      <c r="A83"/>
-      <c r="B83"/>
-    </row>
-    <row r="84" spans="1:2" ht="12.75">
-      <c r="A84"/>
-      <c r="B84"/>
-    </row>
-    <row r="85" spans="1:2" ht="12.75">
-      <c r="A85"/>
-      <c r="B85"/>
-    </row>
-    <row r="86" spans="1:2" ht="12.75">
-      <c r="A86"/>
-      <c r="B86"/>
-    </row>
-    <row r="87" spans="1:2" ht="12.75">
-      <c r="A87"/>
-      <c r="B87"/>
-    </row>
-    <row r="88" spans="1:2" ht="12.75">
-      <c r="A88"/>
-      <c r="B88"/>
-    </row>
-    <row r="89" spans="1:2" ht="12.75">
-      <c r="A89"/>
-      <c r="B89"/>
-    </row>
-    <row r="90" spans="1:2" ht="12.75">
-      <c r="A90"/>
-      <c r="B90"/>
-    </row>
-    <row r="91" spans="1:2" ht="12.75">
-      <c r="A91"/>
-      <c r="B91"/>
-    </row>
-    <row r="92" spans="1:2" ht="12.75">
-      <c r="A92"/>
-      <c r="B92"/>
-    </row>
-    <row r="93" spans="1:2" ht="12.75">
-      <c r="A93"/>
-      <c r="B93"/>
-    </row>
-    <row r="94" spans="1:2" ht="12.75">
-      <c r="A94"/>
-      <c r="B94"/>
-    </row>
-    <row r="95" spans="1:2" ht="12.75">
-      <c r="A95"/>
-      <c r="B95"/>
-    </row>
-    <row r="96" spans="1:2" ht="12.75">
-      <c r="A96"/>
-      <c r="B96"/>
-    </row>
-    <row r="97" spans="1:2" ht="12.75">
-      <c r="A97"/>
-      <c r="B97"/>
-    </row>
-    <row r="98" spans="1:2" ht="12.75">
-      <c r="A98"/>
-      <c r="B98"/>
-    </row>
-    <row r="99" spans="1:2" ht="12.75">
-      <c r="A99"/>
-      <c r="B99"/>
-    </row>
-    <row r="100" spans="1:2" ht="12.75">
-      <c r="A100"/>
-      <c r="B100"/>
-    </row>
-    <row r="101" spans="1:2" ht="12.75">
-      <c r="A101"/>
-      <c r="B101"/>
-    </row>
-    <row r="102" spans="1:2" ht="12.75">
-      <c r="A102"/>
-      <c r="B102"/>
-    </row>
-    <row r="103" spans="1:2" ht="12.75">
-      <c r="A103"/>
-      <c r="B103"/>
-    </row>
-    <row r="104" spans="1:2" ht="12.75">
-      <c r="A104"/>
-      <c r="B104"/>
-    </row>
-    <row r="105" spans="1:2" ht="12.75">
-      <c r="A105"/>
-      <c r="B105"/>
-    </row>
-    <row r="106" spans="1:2" ht="12.75">
-      <c r="A106"/>
-      <c r="B106"/>
-    </row>
-    <row r="107" spans="1:2" ht="12.75">
-      <c r="A107"/>
-      <c r="B107"/>
-    </row>
-    <row r="108" spans="1:2" ht="12.75">
-      <c r="A108"/>
-      <c r="B108"/>
-    </row>
-    <row r="109" spans="1:2" ht="12.75">
-      <c r="A109"/>
-      <c r="B109"/>
-    </row>
-    <row r="110" spans="1:2" ht="12.75">
-      <c r="A110"/>
-      <c r="B110"/>
-    </row>
-    <row r="111" spans="1:2" ht="12.75">
-      <c r="A111"/>
-      <c r="B111"/>
-    </row>
-    <row r="112" spans="1:2" ht="12.75">
-      <c r="A112"/>
-      <c r="B112"/>
-    </row>
-    <row r="113" spans="1:2" ht="12.75">
-      <c r="A113"/>
-      <c r="B113"/>
-    </row>
-    <row r="114" spans="1:2" ht="12.75">
-      <c r="A114"/>
-      <c r="B114"/>
-    </row>
-    <row r="115" spans="1:2" ht="12.75">
-      <c r="A115"/>
-      <c r="B115"/>
-    </row>
-    <row r="116" spans="1:2" ht="12.75">
-      <c r="A116"/>
-      <c r="B116"/>
-    </row>
-    <row r="117" spans="1:2" ht="12.75">
-      <c r="A117"/>
-      <c r="B117"/>
-    </row>
-    <row r="118" spans="1:2" ht="12.75">
-      <c r="A118"/>
-      <c r="B118"/>
-    </row>
-    <row r="119" spans="1:2" ht="12.75">
-      <c r="A119"/>
-      <c r="B119"/>
-    </row>
-    <row r="120" spans="1:2" ht="12.75">
-      <c r="A120"/>
-      <c r="B120"/>
-    </row>
-    <row r="121" spans="1:2" ht="12.75">
-      <c r="A121"/>
-      <c r="B121"/>
-    </row>
-    <row r="122" spans="1:2" ht="12.75">
-      <c r="A122"/>
-      <c r="B122"/>
-    </row>
-    <row r="123" spans="1:2" ht="12.75">
-      <c r="A123"/>
-      <c r="B123"/>
-    </row>
-    <row r="124" spans="1:2" ht="12.75">
-      <c r="A124"/>
-      <c r="B124"/>
-    </row>
-    <row r="125" spans="1:2" ht="12.75">
-      <c r="A125"/>
-      <c r="B125"/>
-    </row>
-    <row r="126" spans="1:2" ht="12.75">
-      <c r="A126"/>
-      <c r="B126"/>
-    </row>
-    <row r="127" spans="1:2" ht="12.75">
-      <c r="A127"/>
-      <c r="B127"/>
-    </row>
-    <row r="128" spans="1:2" ht="12.75">
-      <c r="A128"/>
-      <c r="B128"/>
-    </row>
-    <row r="129" spans="1:2" ht="12.75">
-      <c r="A129"/>
-      <c r="B129"/>
-    </row>
-    <row r="130" spans="1:2" ht="12.75">
-      <c r="A130"/>
-      <c r="B130"/>
-    </row>
-    <row r="131" spans="1:2" ht="12.75">
-      <c r="A131"/>
-      <c r="B131"/>
-    </row>
-    <row r="132" spans="1:2" ht="12.75">
-      <c r="A132"/>
-      <c r="B132"/>
-    </row>
-    <row r="133" spans="1:2" ht="12.75">
-      <c r="A133"/>
-      <c r="B133"/>
-    </row>
-    <row r="134" spans="1:2" ht="12.75">
-      <c r="A134"/>
-      <c r="B134"/>
-    </row>
-    <row r="135" spans="1:2" ht="12.75">
-      <c r="A135"/>
-      <c r="B135"/>
-    </row>
-    <row r="136" spans="1:2" ht="12.75">
-      <c r="A136"/>
-      <c r="B136"/>
-    </row>
-    <row r="137" spans="1:2" ht="12.75">
-      <c r="A137"/>
-      <c r="B137"/>
-    </row>
-    <row r="138" spans="1:2" ht="12.75">
-      <c r="A138"/>
-      <c r="B138"/>
-    </row>
-    <row r="139" spans="1:2" ht="12.75">
-      <c r="A139"/>
-      <c r="B139"/>
-    </row>
-    <row r="140" spans="1:2" ht="12.75">
-      <c r="A140"/>
-      <c r="B140"/>
-    </row>
-    <row r="141" spans="1:2" ht="12.75">
-      <c r="A141"/>
-      <c r="B141"/>
-    </row>
-    <row r="142" spans="1:2" ht="12.75">
-      <c r="A142"/>
-      <c r="B142"/>
-    </row>
-    <row r="143" spans="1:2" ht="12.75">
-      <c r="A143"/>
-      <c r="B143"/>
-    </row>
-    <row r="144" spans="1:2" ht="12.75">
-      <c r="A144"/>
-      <c r="B144"/>
-    </row>
-    <row r="145" spans="1:2" ht="12.75">
-      <c r="A145"/>
-      <c r="B145"/>
-    </row>
-    <row r="146" spans="1:2" ht="12.75">
-      <c r="A146"/>
-      <c r="B146"/>
-    </row>
-    <row r="147" spans="1:2" ht="12.75">
-      <c r="A147"/>
-      <c r="B147"/>
-    </row>
-    <row r="148" spans="1:2" ht="12.75">
-      <c r="A148"/>
-      <c r="B148"/>
-    </row>
-    <row r="149" spans="1:2" ht="12.75">
-      <c r="A149"/>
-      <c r="B149"/>
-    </row>
-    <row r="150" spans="1:2" ht="12.75">
-      <c r="A150"/>
-      <c r="B150"/>
-    </row>
-    <row r="151" spans="1:2" ht="12.75">
-      <c r="A151"/>
-      <c r="B151"/>
-    </row>
-    <row r="152" spans="1:2" ht="12.75">
-      <c r="A152"/>
-      <c r="B152"/>
-    </row>
-    <row r="153" spans="1:2" ht="12.75">
-      <c r="A153"/>
-      <c r="B153"/>
-    </row>
-    <row r="154" spans="1:2" ht="12.75">
-      <c r="A154"/>
-      <c r="B154"/>
-    </row>
-    <row r="155" spans="1:2" ht="12.75">
-      <c r="A155"/>
-      <c r="B155"/>
-    </row>
-    <row r="156" spans="1:2" ht="12.75">
-      <c r="A156"/>
-      <c r="B156"/>
-    </row>
-    <row r="157" spans="1:2" ht="12.75">
-      <c r="A157"/>
-      <c r="B157"/>
-    </row>
-    <row r="158" spans="1:2" ht="12.75">
-      <c r="A158"/>
-      <c r="B158"/>
-    </row>
-    <row r="159" spans="1:2" ht="12.75">
-      <c r="A159"/>
-      <c r="B159"/>
-    </row>
-    <row r="160" spans="1:2" ht="12.75">
-      <c r="A160"/>
-      <c r="B160"/>
-    </row>
-    <row r="161" spans="1:2" ht="12.75">
-      <c r="A161"/>
-      <c r="B161"/>
-    </row>
-    <row r="162" spans="1:2" ht="12.75">
-      <c r="A162"/>
-      <c r="B162"/>
-    </row>
-    <row r="163" spans="1:2" ht="12.75">
-      <c r="A163"/>
-      <c r="B163"/>
-    </row>
-    <row r="164" spans="1:2" ht="12.75">
-      <c r="A164"/>
-      <c r="B164"/>
-    </row>
-    <row r="165" spans="1:2" ht="12.75">
-      <c r="A165"/>
-      <c r="B165"/>
-    </row>
-    <row r="166" spans="1:2" ht="12.75">
-      <c r="A166"/>
-      <c r="B166"/>
-    </row>
-    <row r="167" spans="1:2" thickBot="1">
-      <c r="A167"/>
-      <c r="B167"/>
-    </row>
-    <row r="169" spans="1:2" ht="12.75"/>
-    <row r="170" spans="1:2" ht="12.75"/>
-    <row r="171" spans="1:2" ht="12.75"/>
-    <row r="172" spans="1:2" ht="12.75"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Measuring inconsistencies in Blik
</commit_message>
<xml_diff>
--- a/Blik/Medewerkers.xlsx
+++ b/Blik/Medewerkers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="390" windowWidth="15195" windowHeight="8145"/>
+    <workbookView xWindow="480" yWindow="390" windowWidth="15195" windowHeight="8145" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="medewerkers" sheetId="5" r:id="rId1"/>
@@ -12,6 +12,8 @@
     <sheet name="Dienstverbanden" sheetId="9" r:id="rId3"/>
     <sheet name="WTR" sheetId="10" r:id="rId4"/>
     <sheet name="Teams" sheetId="11" r:id="rId5"/>
+    <sheet name="Blad1" sheetId="12" r:id="rId6"/>
+    <sheet name="Functies" sheetId="13" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">medewerkers!#REF!</definedName>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10097" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10505" uniqueCount="430">
   <si>
     <t>Dhr. A. BAAS</t>
   </si>
@@ -1037,6 +1039,282 @@
   <si>
     <t>Bianca Peters</t>
   </si>
+  <si>
+    <t>Adviseur</t>
+  </si>
+  <si>
+    <t>Bedrijfsvoering</t>
+  </si>
+  <si>
+    <t>BeleidsMedewerker</t>
+  </si>
+  <si>
+    <t>Inspecteur</t>
+  </si>
+  <si>
+    <t>Toezicht</t>
+  </si>
+  <si>
+    <t>Medewerker</t>
+  </si>
+  <si>
+    <t>Administratie</t>
+  </si>
+  <si>
+    <t>Administratie WJ</t>
+  </si>
+  <si>
+    <t>Advisering</t>
+  </si>
+  <si>
+    <t>Behandelen en Ontwikkelen</t>
+  </si>
+  <si>
+    <t>Facilitair Management</t>
+  </si>
+  <si>
+    <t>Facilitair Management WJ</t>
+  </si>
+  <si>
+    <t>ICT</t>
+  </si>
+  <si>
+    <t>ICT/Techniek/Inf.beh./DIV</t>
+  </si>
+  <si>
+    <t>Toezicht WJ</t>
+  </si>
+  <si>
+    <t>Vervoer</t>
+  </si>
+  <si>
+    <t>Verwerken en Behandelen</t>
+  </si>
+  <si>
+    <t>Verwerken en Behandelen WJ</t>
+  </si>
+  <si>
+    <t>OnderzoeksMedewerker</t>
+  </si>
+  <si>
+    <t>Programmadirecteur</t>
+  </si>
+  <si>
+    <t>Programmamanager</t>
+  </si>
+  <si>
+    <t>Coördinerend specialistisch</t>
+  </si>
+  <si>
+    <t>Bedrijven</t>
+  </si>
+  <si>
+    <t>Forensisch</t>
+  </si>
+  <si>
+    <t>Accountant</t>
+  </si>
+  <si>
+    <t>Ondersteunend</t>
+  </si>
+  <si>
+    <t>Operationeel</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Senior</t>
+  </si>
+  <si>
+    <t>Specialistisch</t>
+  </si>
+  <si>
+    <t>Strategisch</t>
+  </si>
+  <si>
+    <t>Wetenschappelijk</t>
+  </si>
+  <si>
+    <t>[Functie]</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>f3</t>
+  </si>
+  <si>
+    <t>f4</t>
+  </si>
+  <si>
+    <t>f5</t>
+  </si>
+  <si>
+    <t>f6</t>
+  </si>
+  <si>
+    <t>f7</t>
+  </si>
+  <si>
+    <t>f8</t>
+  </si>
+  <si>
+    <t>f9</t>
+  </si>
+  <si>
+    <t>f10</t>
+  </si>
+  <si>
+    <t>f11</t>
+  </si>
+  <si>
+    <t>f12</t>
+  </si>
+  <si>
+    <t>f13</t>
+  </si>
+  <si>
+    <t>f14</t>
+  </si>
+  <si>
+    <t>f15</t>
+  </si>
+  <si>
+    <t>f16</t>
+  </si>
+  <si>
+    <t>f17</t>
+  </si>
+  <si>
+    <t>f18</t>
+  </si>
+  <si>
+    <t>f19</t>
+  </si>
+  <si>
+    <t>f20</t>
+  </si>
+  <si>
+    <t>f21</t>
+  </si>
+  <si>
+    <t>f22</t>
+  </si>
+  <si>
+    <t>f23</t>
+  </si>
+  <si>
+    <t>f24</t>
+  </si>
+  <si>
+    <t>f25</t>
+  </si>
+  <si>
+    <t>f26</t>
+  </si>
+  <si>
+    <t>f27</t>
+  </si>
+  <si>
+    <t>f28</t>
+  </si>
+  <si>
+    <t>f29</t>
+  </si>
+  <si>
+    <t>f30</t>
+  </si>
+  <si>
+    <t>f31</t>
+  </si>
+  <si>
+    <t>f32</t>
+  </si>
+  <si>
+    <t>f33</t>
+  </si>
+  <si>
+    <t>f34</t>
+  </si>
+  <si>
+    <t>f35</t>
+  </si>
+  <si>
+    <t>f36</t>
+  </si>
+  <si>
+    <t>f37</t>
+  </si>
+  <si>
+    <t>f38</t>
+  </si>
+  <si>
+    <t>f39</t>
+  </si>
+  <si>
+    <t>f40</t>
+  </si>
+  <si>
+    <t>f41</t>
+  </si>
+  <si>
+    <t>f42</t>
+  </si>
+  <si>
+    <t>f43</t>
+  </si>
+  <si>
+    <t>f44</t>
+  </si>
+  <si>
+    <t>f45</t>
+  </si>
+  <si>
+    <t>f46</t>
+  </si>
+  <si>
+    <t>f47</t>
+  </si>
+  <si>
+    <t>functienaam</t>
+  </si>
+  <si>
+    <t>functiekwal</t>
+  </si>
+  <si>
+    <t>functiegebied</t>
+  </si>
+  <si>
+    <t>Kwalificatie</t>
+  </si>
+  <si>
+    <t>Functienaam</t>
+  </si>
+  <si>
+    <t>Functiegebied</t>
+  </si>
+  <si>
+    <t>f31,f32</t>
+  </si>
+  <si>
+    <t>f29,f30</t>
+  </si>
+  <si>
+    <t>f10,f11</t>
+  </si>
+  <si>
+    <t>f13,f14</t>
+  </si>
+  <si>
+    <t>f13,f31</t>
+  </si>
+  <si>
+    <t>f16,f43</t>
+  </si>
 </sst>
 </file>
 
@@ -1522,7 +1800,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1559,6 +1837,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1903,7 +2182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -2420,7 +2699,7 @@
   <dimension ref="A1:D3361"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -78915,4 +79194,2152 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="6" max="6" width="44.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17" t="s">
+        <v>419</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>418</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="C2" t="str">
+        <f>VLOOKUP(B2,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> 99999999 </v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>421</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>422</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="C3" t="str">
+        <f>VLOOKUP(B3,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Adviseur </v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="F3" t="str">
+        <f>G3&amp;" "&amp;H3&amp;" "&amp;I3</f>
+        <v xml:space="preserve"> 99999999 </v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>426</v>
+      </c>
+      <c r="C4" t="e">
+        <f>VLOOKUP(B4,E$3:F$49,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="F4" t="str">
+        <f>G4&amp;" "&amp;H4&amp;" "&amp;I4</f>
+        <v xml:space="preserve">Forensisch Accountant </v>
+      </c>
+      <c r="G4" t="s">
+        <v>361</v>
+      </c>
+      <c r="H4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="C5" t="str">
+        <f>VLOOKUP(B5,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Adviseur Bedrijfsvoering</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="F5" t="str">
+        <f>G5&amp;" "&amp;H5&amp;" "&amp;I5</f>
+        <v xml:space="preserve"> Adviseur Bedrijfsvoering</v>
+      </c>
+      <c r="H5" t="s">
+        <v>338</v>
+      </c>
+      <c r="I5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A6" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="C6" t="str">
+        <f>VLOOKUP(B6,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Beleidsondersteuner </v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="F6" t="str">
+        <f>G6&amp;" "&amp;H6&amp;" "&amp;I6</f>
+        <v>Senior Adviseur Bedrijfsvoering</v>
+      </c>
+      <c r="G6" t="s">
+        <v>366</v>
+      </c>
+      <c r="H6" t="s">
+        <v>338</v>
+      </c>
+      <c r="I6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="C7" t="str">
+        <f>VLOOKUP(B7,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Coördinerend specialistisch Adviseur </v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="F7" t="str">
+        <f>G7&amp;" "&amp;H7&amp;" "&amp;I7</f>
+        <v>Coördinerend specialistisch Adviseur Bedrijven</v>
+      </c>
+      <c r="G7" t="s">
+        <v>359</v>
+      </c>
+      <c r="H7" t="s">
+        <v>338</v>
+      </c>
+      <c r="I7" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A8" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="C8" t="str">
+        <f>VLOOKUP(B8,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Coördinerend specialistisch Adviseur </v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="F8" t="str">
+        <f>G8&amp;" "&amp;H8&amp;" "&amp;I8</f>
+        <v xml:space="preserve"> Adviseur </v>
+      </c>
+      <c r="H8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="C9" t="str">
+        <f>VLOOKUP(B9,E$3:F$49,2,FALSE)</f>
+        <v>Coördinerend specialistisch Adviseur Bedrijven</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="F9" t="str">
+        <f>G9&amp;" "&amp;H9&amp;" "&amp;I9</f>
+        <v xml:space="preserve">Coördinerend specialistisch Adviseur </v>
+      </c>
+      <c r="G9" t="s">
+        <v>359</v>
+      </c>
+      <c r="H9" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A10" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="C10" t="str">
+        <f>VLOOKUP(B10,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Coördinerend specialistisch Inspecteur </v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="F10" t="str">
+        <f>G10&amp;" "&amp;H10&amp;" "&amp;I10</f>
+        <v xml:space="preserve">Senior Adviseur </v>
+      </c>
+      <c r="G10" t="s">
+        <v>366</v>
+      </c>
+      <c r="H10" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A11" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="C11" t="str">
+        <f>VLOOKUP(B11,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Coördinerend specialistisch Inspecteur </v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="F11" t="str">
+        <f>G11&amp;" "&amp;H11&amp;" "&amp;I11</f>
+        <v xml:space="preserve">Specialistisch Adviseur </v>
+      </c>
+      <c r="G11" t="s">
+        <v>367</v>
+      </c>
+      <c r="H11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="C12" t="str">
+        <f>VLOOKUP(B12,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Coördinerend specialistisch Adviseur </v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>380</v>
+      </c>
+      <c r="F12" t="str">
+        <f>G12&amp;" "&amp;H12&amp;" "&amp;I12</f>
+        <v xml:space="preserve"> BeleidsMedewerker </v>
+      </c>
+      <c r="H12" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A13" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="C13" t="str">
+        <f>VLOOKUP(B13,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Coördinerend specialistisch Inspecteur </v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="F13" t="str">
+        <f>G13&amp;" "&amp;H13&amp;" "&amp;I13</f>
+        <v xml:space="preserve">Senior BeleidsMedewerker </v>
+      </c>
+      <c r="G13" t="s">
+        <v>366</v>
+      </c>
+      <c r="H13" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A14" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="C14" t="str">
+        <f>VLOOKUP(B14,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Coördinerend specialistisch Medewerker </v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="F14" t="str">
+        <f>G14&amp;" "&amp;H14&amp;" "&amp;I14</f>
+        <v xml:space="preserve"> Beleidsondersteuner </v>
+      </c>
+      <c r="H14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="C15" t="str">
+        <f>VLOOKUP(B15,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Externe Medewerker </v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="F15" t="str">
+        <f>G15&amp;" "&amp;H15&amp;" "&amp;I15</f>
+        <v xml:space="preserve"> Inspecteur Toezicht</v>
+      </c>
+      <c r="H15" t="s">
+        <v>341</v>
+      </c>
+      <c r="I15" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="C16" t="str">
+        <f>VLOOKUP(B16,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Externe Medewerker </v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="F16" t="str">
+        <f>G16&amp;" "&amp;H16&amp;" "&amp;I16</f>
+        <v xml:space="preserve"> Inspecteur </v>
+      </c>
+      <c r="H16" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A17" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="C17" t="str">
+        <f>VLOOKUP(B17,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Forensisch Accountant </v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="F17" t="str">
+        <f>G17&amp;" "&amp;H17&amp;" "&amp;I17</f>
+        <v xml:space="preserve">Coördinerend specialistisch Inspecteur </v>
+      </c>
+      <c r="G17" t="s">
+        <v>359</v>
+      </c>
+      <c r="H17" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="C18" t="str">
+        <f>VLOOKUP(B18,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Inspecteur Generaal </v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="F18" t="str">
+        <f>G18&amp;" "&amp;H18&amp;" "&amp;I18</f>
+        <v xml:space="preserve">Senior Inspecteur </v>
+      </c>
+      <c r="G18" t="s">
+        <v>366</v>
+      </c>
+      <c r="H18" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>427</v>
+      </c>
+      <c r="C19" t="e">
+        <f>VLOOKUP(B19,E$3:F$49,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="F19" t="str">
+        <f>G19&amp;" "&amp;H19&amp;" "&amp;I19</f>
+        <v xml:space="preserve">Strategisch Inspecteur </v>
+      </c>
+      <c r="G19" t="s">
+        <v>368</v>
+      </c>
+      <c r="H19" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A20" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>428</v>
+      </c>
+      <c r="C20" t="e">
+        <f>VLOOKUP(B20,E$3:F$49,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="F20" t="str">
+        <f>G20&amp;" "&amp;H20&amp;" "&amp;I20</f>
+        <v xml:space="preserve"> Inspecteur Generaal </v>
+      </c>
+      <c r="H20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>389</v>
+      </c>
+      <c r="C21" t="str">
+        <f>VLOOKUP(B21,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Managementondersteuner </v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>389</v>
+      </c>
+      <c r="F21" t="str">
+        <f>G21&amp;" "&amp;H21&amp;" "&amp;I21</f>
+        <v xml:space="preserve"> Managementondersteuner </v>
+      </c>
+      <c r="H21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A22" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>404</v>
+      </c>
+      <c r="C22" t="str">
+        <f>VLOOKUP(B22,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Verwerken en Behandelen</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>390</v>
+      </c>
+      <c r="F22" t="str">
+        <f>G22&amp;" "&amp;H22&amp;" "&amp;I22</f>
+        <v xml:space="preserve">Operationeel Manager </v>
+      </c>
+      <c r="G22" t="s">
+        <v>364</v>
+      </c>
+      <c r="H22" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A23" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>405</v>
+      </c>
+      <c r="C23" t="str">
+        <f>VLOOKUP(B23,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Verwerken en Behandelen WJ</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>391</v>
+      </c>
+      <c r="F23" t="str">
+        <f>G23&amp;" "&amp;H23&amp;" "&amp;I23</f>
+        <v xml:space="preserve"> Medewerker Administratie</v>
+      </c>
+      <c r="H23" t="s">
+        <v>343</v>
+      </c>
+      <c r="I23" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>391</v>
+      </c>
+      <c r="C24" t="str">
+        <f>VLOOKUP(B24,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Administratie</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="F24" t="str">
+        <f>G24&amp;" "&amp;H24&amp;" "&amp;I24</f>
+        <v xml:space="preserve"> Medewerker Administratie WJ</v>
+      </c>
+      <c r="H24" t="s">
+        <v>343</v>
+      </c>
+      <c r="I24" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A25" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="C25" t="str">
+        <f>VLOOKUP(B25,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Administratie WJ</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="F25" t="str">
+        <f>G25&amp;" "&amp;H25&amp;" "&amp;I25</f>
+        <v xml:space="preserve"> Medewerker Advisering</v>
+      </c>
+      <c r="H25" t="s">
+        <v>343</v>
+      </c>
+      <c r="I25" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A26" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="C26" t="str">
+        <f>VLOOKUP(B26,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Administratie WJ</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>394</v>
+      </c>
+      <c r="F26" t="str">
+        <f>G26&amp;" "&amp;H26&amp;" "&amp;I26</f>
+        <v xml:space="preserve"> Medewerker Behandelen en Ontwikkelen</v>
+      </c>
+      <c r="H26" t="s">
+        <v>343</v>
+      </c>
+      <c r="I26" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A27" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="C27" t="str">
+        <f>VLOOKUP(B27,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Administratie WJ</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>395</v>
+      </c>
+      <c r="F27" t="str">
+        <f>G27&amp;" "&amp;H27&amp;" "&amp;I27</f>
+        <v xml:space="preserve"> Medewerker Facilitair Management</v>
+      </c>
+      <c r="H27" t="s">
+        <v>343</v>
+      </c>
+      <c r="I27" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A28" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="C28" t="str">
+        <f>VLOOKUP(B28,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Advisering</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>396</v>
+      </c>
+      <c r="F28" t="str">
+        <f>G28&amp;" "&amp;H28&amp;" "&amp;I28</f>
+        <v xml:space="preserve"> Medewerker Facilitair Management WJ</v>
+      </c>
+      <c r="H28" t="s">
+        <v>343</v>
+      </c>
+      <c r="I28" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>394</v>
+      </c>
+      <c r="C29" t="str">
+        <f>VLOOKUP(B29,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Behandelen en Ontwikkelen</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>397</v>
+      </c>
+      <c r="F29" t="str">
+        <f>G29&amp;" "&amp;H29&amp;" "&amp;I29</f>
+        <v xml:space="preserve"> Medewerker ICT</v>
+      </c>
+      <c r="H29" t="s">
+        <v>343</v>
+      </c>
+      <c r="I29" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>395</v>
+      </c>
+      <c r="C30" t="str">
+        <f>VLOOKUP(B30,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Facilitair Management</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="F30" t="str">
+        <f>G30&amp;" "&amp;H30&amp;" "&amp;I30</f>
+        <v xml:space="preserve"> Medewerker ICT/Techniek/Inf.beh./DIV</v>
+      </c>
+      <c r="H30" t="s">
+        <v>343</v>
+      </c>
+      <c r="I30" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A31" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>396</v>
+      </c>
+      <c r="C31" t="str">
+        <f>VLOOKUP(B31,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Facilitair Management WJ</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>399</v>
+      </c>
+      <c r="F31" t="str">
+        <f>G31&amp;" "&amp;H31&amp;" "&amp;I31</f>
+        <v xml:space="preserve"> Medewerker Toezicht</v>
+      </c>
+      <c r="H31" t="s">
+        <v>343</v>
+      </c>
+      <c r="I31" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A32" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>397</v>
+      </c>
+      <c r="C32" t="str">
+        <f>VLOOKUP(B32,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker ICT</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="F32" t="str">
+        <f>G32&amp;" "&amp;H32&amp;" "&amp;I32</f>
+        <v>Ondersteunend Medewerker Toezicht</v>
+      </c>
+      <c r="G32" t="s">
+        <v>363</v>
+      </c>
+      <c r="H32" t="s">
+        <v>343</v>
+      </c>
+      <c r="I32" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A33" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="C33" t="str">
+        <f>VLOOKUP(B33,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker ICT/Techniek/Inf.beh./DIV</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>401</v>
+      </c>
+      <c r="F33" t="str">
+        <f>G33&amp;" "&amp;H33&amp;" "&amp;I33</f>
+        <v xml:space="preserve"> Medewerker Toezicht WJ</v>
+      </c>
+      <c r="H33" t="s">
+        <v>343</v>
+      </c>
+      <c r="I33" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A34" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>403</v>
+      </c>
+      <c r="C34" t="str">
+        <f>VLOOKUP(B34,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Vervoer</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>402</v>
+      </c>
+      <c r="F34" t="str">
+        <f>G34&amp;" "&amp;H34&amp;" "&amp;I34</f>
+        <v>Ondersteunend Medewerker Toezicht WJ</v>
+      </c>
+      <c r="G34" t="s">
+        <v>363</v>
+      </c>
+      <c r="H34" t="s">
+        <v>343</v>
+      </c>
+      <c r="I34" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>404</v>
+      </c>
+      <c r="C35" t="str">
+        <f>VLOOKUP(B35,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Verwerken en Behandelen</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>403</v>
+      </c>
+      <c r="F35" t="str">
+        <f>G35&amp;" "&amp;H35&amp;" "&amp;I35</f>
+        <v xml:space="preserve"> Medewerker Vervoer</v>
+      </c>
+      <c r="H35" t="s">
+        <v>343</v>
+      </c>
+      <c r="I35" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A36" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>405</v>
+      </c>
+      <c r="C36" t="str">
+        <f>VLOOKUP(B36,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Verwerken en Behandelen WJ</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>404</v>
+      </c>
+      <c r="F36" t="str">
+        <f>G36&amp;" "&amp;H36&amp;" "&amp;I36</f>
+        <v xml:space="preserve"> Medewerker Verwerken en Behandelen</v>
+      </c>
+      <c r="H36" t="s">
+        <v>343</v>
+      </c>
+      <c r="I36" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A37" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>405</v>
+      </c>
+      <c r="C37" t="str">
+        <f>VLOOKUP(B37,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Verwerken en Behandelen WJ</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>405</v>
+      </c>
+      <c r="F37" t="str">
+        <f>G37&amp;" "&amp;H37&amp;" "&amp;I37</f>
+        <v xml:space="preserve"> Medewerker Verwerken en Behandelen WJ</v>
+      </c>
+      <c r="H37" t="s">
+        <v>343</v>
+      </c>
+      <c r="I37" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A38" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>404</v>
+      </c>
+      <c r="C38" t="str">
+        <f>VLOOKUP(B38,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Medewerker Verwerken en Behandelen</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="F38" t="str">
+        <f>G38&amp;" "&amp;H38&amp;" "&amp;I38</f>
+        <v xml:space="preserve">Coördinerend specialistisch Medewerker </v>
+      </c>
+      <c r="G38" t="s">
+        <v>359</v>
+      </c>
+      <c r="H38" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A39" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="C39" t="str">
+        <f>VLOOKUP(B39,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Middenmanager </v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="F39" t="str">
+        <f>G39&amp;" "&amp;H39&amp;" "&amp;I39</f>
+        <v xml:space="preserve">Externe Medewerker </v>
+      </c>
+      <c r="G39" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A40" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="C40" t="str">
+        <f>VLOOKUP(B40,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Middenmanager </v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>408</v>
+      </c>
+      <c r="F40" t="str">
+        <f>G40&amp;" "&amp;H40&amp;" "&amp;I40</f>
+        <v xml:space="preserve">Wetenschappelijk Medewerker </v>
+      </c>
+      <c r="G40" t="s">
+        <v>369</v>
+      </c>
+      <c r="H40" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A41" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" t="e">
+        <f>VLOOKUP(B41,E$3:F$49,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="F41" t="str">
+        <f>G41&amp;" "&amp;H41&amp;" "&amp;I41</f>
+        <v xml:space="preserve"> Middenmanager </v>
+      </c>
+      <c r="H41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A42" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="C42" t="e">
+        <f>VLOOKUP(B42,E$3:F$49,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="F42" t="str">
+        <f>G42&amp;" "&amp;H42&amp;" "&amp;I42</f>
+        <v xml:space="preserve"> OnderzoeksMedewerker </v>
+      </c>
+      <c r="H42" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A43" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>424</v>
+      </c>
+      <c r="C43" t="e">
+        <f>VLOOKUP(B43,E$3:F$49,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="F43" t="str">
+        <f>G43&amp;" "&amp;H43&amp;" "&amp;I43</f>
+        <v xml:space="preserve"> Onderzoeksondersteuner </v>
+      </c>
+      <c r="H43" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A44" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="C44" t="e">
+        <f>VLOOKUP(B44,E$3:F$49,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>412</v>
+      </c>
+      <c r="F44" t="str">
+        <f>G44&amp;" "&amp;H44&amp;" "&amp;I44</f>
+        <v xml:space="preserve"> Practitioner </v>
+      </c>
+      <c r="H44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A45" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="C45" t="e">
+        <f>VLOOKUP(B45,E$3:F$49,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="F45" t="str">
+        <f>G45&amp;" "&amp;H45&amp;" "&amp;I45</f>
+        <v xml:space="preserve">Senior Practitioner </v>
+      </c>
+      <c r="G45" t="s">
+        <v>366</v>
+      </c>
+      <c r="H45" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A46" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>424</v>
+      </c>
+      <c r="C46" t="e">
+        <f>VLOOKUP(B46,E$3:F$49,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>414</v>
+      </c>
+      <c r="F46" t="str">
+        <f>G46&amp;" "&amp;H46&amp;" "&amp;I46</f>
+        <v xml:space="preserve"> Programmadirecteur </v>
+      </c>
+      <c r="H46" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A47" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="C47" t="e">
+        <f>VLOOKUP(B47,E$3:F$49,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>415</v>
+      </c>
+      <c r="F47" t="str">
+        <f>G47&amp;" "&amp;H47&amp;" "&amp;I47</f>
+        <v xml:space="preserve"> Programmamanager </v>
+      </c>
+      <c r="H47" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A48" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="C48" t="e">
+        <f>VLOOKUP(B48,E$3:F$49,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>416</v>
+      </c>
+      <c r="F48" t="str">
+        <f>G48&amp;" "&amp;H48&amp;" "&amp;I48</f>
+        <v xml:space="preserve"> Stagiair </v>
+      </c>
+      <c r="H48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A49" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="C49" t="e">
+        <f>VLOOKUP(B49,E$3:F$49,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="F49" t="str">
+        <f>G49&amp;" "&amp;H49&amp;" "&amp;I49</f>
+        <v xml:space="preserve"> Topmanager </v>
+      </c>
+      <c r="H49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A50" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="C50" t="str">
+        <f>VLOOKUP(B50,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Onderzoeksondersteuner </v>
+      </c>
+      <c r="E50" s="17"/>
+    </row>
+    <row r="51" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A51" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="C51" t="str">
+        <f>VLOOKUP(B51,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> OnderzoeksMedewerker </v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A52" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="C52" t="str">
+        <f>VLOOKUP(B52,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Onderzoeksondersteuner </v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A53" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>390</v>
+      </c>
+      <c r="C53" t="str">
+        <f>VLOOKUP(B53,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Operationeel Manager </v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A54" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>412</v>
+      </c>
+      <c r="C54" t="str">
+        <f>VLOOKUP(B54,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Practitioner </v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A55" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>414</v>
+      </c>
+      <c r="C55" t="str">
+        <f>VLOOKUP(B55,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Programmadirecteur </v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A56" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>415</v>
+      </c>
+      <c r="C56" t="str">
+        <f>VLOOKUP(B56,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Programmamanager </v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A57" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="C57" t="str">
+        <f>VLOOKUP(B57,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Senior Adviseur </v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A58" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="C58" t="str">
+        <f>VLOOKUP(B58,E$3:F$49,2,FALSE)</f>
+        <v>Senior Adviseur Bedrijfsvoering</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A59" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="C59" t="str">
+        <f>VLOOKUP(B59,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Senior BeleidsMedewerker </v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A60" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="C60" t="str">
+        <f>VLOOKUP(B60,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Senior Inspecteur </v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A61" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>429</v>
+      </c>
+      <c r="C61" t="e">
+        <f>VLOOKUP(B61,E$3:F$49,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A62" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="C62" t="str">
+        <f>VLOOKUP(B62,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Specialistisch Adviseur </v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A63" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>416</v>
+      </c>
+      <c r="C63" t="str">
+        <f>VLOOKUP(B63,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Stagiair </v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A64" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>416</v>
+      </c>
+      <c r="C64" t="str">
+        <f>VLOOKUP(B64,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Stagiair </v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="13.5" thickBot="1">
+      <c r="A65" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="C65" t="str">
+        <f>VLOOKUP(B65,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Strategisch Inspecteur </v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="13.5" thickBot="1">
+      <c r="A66" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="C66" t="str">
+        <f>VLOOKUP(B66,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve"> Topmanager </v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="13.5" thickBot="1">
+      <c r="A67" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>408</v>
+      </c>
+      <c r="C67" t="str">
+        <f>VLOOKUP(B67,E$3:F$49,2,FALSE)</f>
+        <v xml:space="preserve">Wetenschappelijk Medewerker </v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="E4:I49">
+    <sortCondition ref="F4:F49"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection sqref="A1:E49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17" t="s">
+        <v>419</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>418</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17" t="s">
+        <v>421</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>422</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="B3" t="str">
+        <f>C3&amp;" "&amp;D3&amp;" "&amp;E3</f>
+        <v xml:space="preserve"> 99999999 </v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="B4" t="str">
+        <f>C4&amp;" "&amp;D4&amp;" "&amp;E4</f>
+        <v xml:space="preserve">Forensisch Accountant </v>
+      </c>
+      <c r="C4" t="s">
+        <v>361</v>
+      </c>
+      <c r="D4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="B5" t="str">
+        <f>C5&amp;" "&amp;D5&amp;" "&amp;E5</f>
+        <v xml:space="preserve"> Adviseur Bedrijfsvoering</v>
+      </c>
+      <c r="D5" t="s">
+        <v>338</v>
+      </c>
+      <c r="E5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="B6" t="str">
+        <f>C6&amp;" "&amp;D6&amp;" "&amp;E6</f>
+        <v>Senior Adviseur Bedrijfsvoering</v>
+      </c>
+      <c r="C6" t="s">
+        <v>366</v>
+      </c>
+      <c r="D6" t="s">
+        <v>338</v>
+      </c>
+      <c r="E6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="B7" t="str">
+        <f>C7&amp;" "&amp;D7&amp;" "&amp;E7</f>
+        <v>Coördinerend specialistisch Adviseur Bedrijven</v>
+      </c>
+      <c r="C7" t="s">
+        <v>359</v>
+      </c>
+      <c r="D7" t="s">
+        <v>338</v>
+      </c>
+      <c r="E7" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="B8" t="str">
+        <f>C8&amp;" "&amp;D8&amp;" "&amp;E8</f>
+        <v xml:space="preserve"> Adviseur </v>
+      </c>
+      <c r="D8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="B9" t="str">
+        <f>C9&amp;" "&amp;D9&amp;" "&amp;E9</f>
+        <v xml:space="preserve">Coördinerend specialistisch Adviseur </v>
+      </c>
+      <c r="C9" t="s">
+        <v>359</v>
+      </c>
+      <c r="D9" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="B10" t="str">
+        <f>C10&amp;" "&amp;D10&amp;" "&amp;E10</f>
+        <v xml:space="preserve">Senior Adviseur </v>
+      </c>
+      <c r="C10" t="s">
+        <v>366</v>
+      </c>
+      <c r="D10" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="B11" t="str">
+        <f>C11&amp;" "&amp;D11&amp;" "&amp;E11</f>
+        <v xml:space="preserve">Specialistisch Adviseur </v>
+      </c>
+      <c r="C11" t="s">
+        <v>367</v>
+      </c>
+      <c r="D11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="17" t="s">
+        <v>380</v>
+      </c>
+      <c r="B12" t="str">
+        <f>C12&amp;" "&amp;D12&amp;" "&amp;E12</f>
+        <v xml:space="preserve"> BeleidsMedewerker </v>
+      </c>
+      <c r="D12" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="B13" t="str">
+        <f>C13&amp;" "&amp;D13&amp;" "&amp;E13</f>
+        <v xml:space="preserve">Senior BeleidsMedewerker </v>
+      </c>
+      <c r="C13" t="s">
+        <v>366</v>
+      </c>
+      <c r="D13" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="B14" t="str">
+        <f>C14&amp;" "&amp;D14&amp;" "&amp;E14</f>
+        <v xml:space="preserve"> Beleidsondersteuner </v>
+      </c>
+      <c r="D14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="B15" t="str">
+        <f>C15&amp;" "&amp;D15&amp;" "&amp;E15</f>
+        <v xml:space="preserve"> Inspecteur Toezicht</v>
+      </c>
+      <c r="D15" t="s">
+        <v>341</v>
+      </c>
+      <c r="E15" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="B16" t="str">
+        <f>C16&amp;" "&amp;D16&amp;" "&amp;E16</f>
+        <v xml:space="preserve"> Inspecteur </v>
+      </c>
+      <c r="D16" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="B17" t="str">
+        <f>C17&amp;" "&amp;D17&amp;" "&amp;E17</f>
+        <v xml:space="preserve">Coördinerend specialistisch Inspecteur </v>
+      </c>
+      <c r="C17" t="s">
+        <v>359</v>
+      </c>
+      <c r="D17" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="B18" t="str">
+        <f>C18&amp;" "&amp;D18&amp;" "&amp;E18</f>
+        <v xml:space="preserve">Senior Inspecteur </v>
+      </c>
+      <c r="C18" t="s">
+        <v>366</v>
+      </c>
+      <c r="D18" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="B19" t="str">
+        <f>C19&amp;" "&amp;D19&amp;" "&amp;E19</f>
+        <v xml:space="preserve">Strategisch Inspecteur </v>
+      </c>
+      <c r="C19" t="s">
+        <v>368</v>
+      </c>
+      <c r="D19" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="B20" t="str">
+        <f>C20&amp;" "&amp;D20&amp;" "&amp;E20</f>
+        <v xml:space="preserve"> Inspecteur Generaal </v>
+      </c>
+      <c r="D20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="17" t="s">
+        <v>389</v>
+      </c>
+      <c r="B21" t="str">
+        <f>C21&amp;" "&amp;D21&amp;" "&amp;E21</f>
+        <v xml:space="preserve"> Managementondersteuner </v>
+      </c>
+      <c r="D21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="17" t="s">
+        <v>390</v>
+      </c>
+      <c r="B22" t="str">
+        <f>C22&amp;" "&amp;D22&amp;" "&amp;E22</f>
+        <v xml:space="preserve">Operationeel Manager </v>
+      </c>
+      <c r="C22" t="s">
+        <v>364</v>
+      </c>
+      <c r="D22" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="17" t="s">
+        <v>391</v>
+      </c>
+      <c r="B23" t="str">
+        <f>C23&amp;" "&amp;D23&amp;" "&amp;E23</f>
+        <v xml:space="preserve"> Medewerker Administratie</v>
+      </c>
+      <c r="D23" t="s">
+        <v>343</v>
+      </c>
+      <c r="E23" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="B24" t="str">
+        <f>C24&amp;" "&amp;D24&amp;" "&amp;E24</f>
+        <v xml:space="preserve"> Medewerker Administratie WJ</v>
+      </c>
+      <c r="D24" t="s">
+        <v>343</v>
+      </c>
+      <c r="E24" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="B25" t="str">
+        <f>C25&amp;" "&amp;D25&amp;" "&amp;E25</f>
+        <v xml:space="preserve"> Medewerker Advisering</v>
+      </c>
+      <c r="D25" t="s">
+        <v>343</v>
+      </c>
+      <c r="E25" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="17" t="s">
+        <v>394</v>
+      </c>
+      <c r="B26" t="str">
+        <f>C26&amp;" "&amp;D26&amp;" "&amp;E26</f>
+        <v xml:space="preserve"> Medewerker Behandelen en Ontwikkelen</v>
+      </c>
+      <c r="D26" t="s">
+        <v>343</v>
+      </c>
+      <c r="E26" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="17" t="s">
+        <v>395</v>
+      </c>
+      <c r="B27" t="str">
+        <f>C27&amp;" "&amp;D27&amp;" "&amp;E27</f>
+        <v xml:space="preserve"> Medewerker Facilitair Management</v>
+      </c>
+      <c r="D27" t="s">
+        <v>343</v>
+      </c>
+      <c r="E27" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="17" t="s">
+        <v>396</v>
+      </c>
+      <c r="B28" t="str">
+        <f>C28&amp;" "&amp;D28&amp;" "&amp;E28</f>
+        <v xml:space="preserve"> Medewerker Facilitair Management WJ</v>
+      </c>
+      <c r="D28" t="s">
+        <v>343</v>
+      </c>
+      <c r="E28" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="17" t="s">
+        <v>397</v>
+      </c>
+      <c r="B29" t="str">
+        <f>C29&amp;" "&amp;D29&amp;" "&amp;E29</f>
+        <v xml:space="preserve"> Medewerker ICT</v>
+      </c>
+      <c r="D29" t="s">
+        <v>343</v>
+      </c>
+      <c r="E29" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="B30" t="str">
+        <f>C30&amp;" "&amp;D30&amp;" "&amp;E30</f>
+        <v xml:space="preserve"> Medewerker ICT/Techniek/Inf.beh./DIV</v>
+      </c>
+      <c r="D30" t="s">
+        <v>343</v>
+      </c>
+      <c r="E30" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="17" t="s">
+        <v>399</v>
+      </c>
+      <c r="B31" t="str">
+        <f>C31&amp;" "&amp;D31&amp;" "&amp;E31</f>
+        <v xml:space="preserve"> Medewerker Toezicht</v>
+      </c>
+      <c r="D31" t="s">
+        <v>343</v>
+      </c>
+      <c r="E31" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B32" t="str">
+        <f>C32&amp;" "&amp;D32&amp;" "&amp;E32</f>
+        <v>Ondersteunend Medewerker Toezicht</v>
+      </c>
+      <c r="C32" t="s">
+        <v>363</v>
+      </c>
+      <c r="D32" t="s">
+        <v>343</v>
+      </c>
+      <c r="E32" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="17" t="s">
+        <v>401</v>
+      </c>
+      <c r="B33" t="str">
+        <f>C33&amp;" "&amp;D33&amp;" "&amp;E33</f>
+        <v xml:space="preserve"> Medewerker Toezicht WJ</v>
+      </c>
+      <c r="D33" t="s">
+        <v>343</v>
+      </c>
+      <c r="E33" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="17" t="s">
+        <v>402</v>
+      </c>
+      <c r="B34" t="str">
+        <f>C34&amp;" "&amp;D34&amp;" "&amp;E34</f>
+        <v>Ondersteunend Medewerker Toezicht WJ</v>
+      </c>
+      <c r="C34" t="s">
+        <v>363</v>
+      </c>
+      <c r="D34" t="s">
+        <v>343</v>
+      </c>
+      <c r="E34" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="17" t="s">
+        <v>403</v>
+      </c>
+      <c r="B35" t="str">
+        <f>C35&amp;" "&amp;D35&amp;" "&amp;E35</f>
+        <v xml:space="preserve"> Medewerker Vervoer</v>
+      </c>
+      <c r="D35" t="s">
+        <v>343</v>
+      </c>
+      <c r="E35" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="17" t="s">
+        <v>404</v>
+      </c>
+      <c r="B36" t="str">
+        <f>C36&amp;" "&amp;D36&amp;" "&amp;E36</f>
+        <v xml:space="preserve"> Medewerker Verwerken en Behandelen</v>
+      </c>
+      <c r="D36" t="s">
+        <v>343</v>
+      </c>
+      <c r="E36" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="17" t="s">
+        <v>405</v>
+      </c>
+      <c r="B37" t="str">
+        <f>C37&amp;" "&amp;D37&amp;" "&amp;E37</f>
+        <v xml:space="preserve"> Medewerker Verwerken en Behandelen WJ</v>
+      </c>
+      <c r="D37" t="s">
+        <v>343</v>
+      </c>
+      <c r="E37" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="B38" t="str">
+        <f>C38&amp;" "&amp;D38&amp;" "&amp;E38</f>
+        <v xml:space="preserve">Coördinerend specialistisch Medewerker </v>
+      </c>
+      <c r="C38" t="s">
+        <v>359</v>
+      </c>
+      <c r="D38" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="B39" t="str">
+        <f>C39&amp;" "&amp;D39&amp;" "&amp;E39</f>
+        <v xml:space="preserve">Externe Medewerker </v>
+      </c>
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="17" t="s">
+        <v>408</v>
+      </c>
+      <c r="B40" t="str">
+        <f>C40&amp;" "&amp;D40&amp;" "&amp;E40</f>
+        <v xml:space="preserve">Wetenschappelijk Medewerker </v>
+      </c>
+      <c r="C40" t="s">
+        <v>369</v>
+      </c>
+      <c r="D40" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="B41" t="str">
+        <f>C41&amp;" "&amp;D41&amp;" "&amp;E41</f>
+        <v xml:space="preserve"> Middenmanager </v>
+      </c>
+      <c r="D41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="B42" t="str">
+        <f>C42&amp;" "&amp;D42&amp;" "&amp;E42</f>
+        <v xml:space="preserve"> OnderzoeksMedewerker </v>
+      </c>
+      <c r="D42" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="B43" t="str">
+        <f>C43&amp;" "&amp;D43&amp;" "&amp;E43</f>
+        <v xml:space="preserve"> Onderzoeksondersteuner </v>
+      </c>
+      <c r="D43" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="17" t="s">
+        <v>412</v>
+      </c>
+      <c r="B44" t="str">
+        <f>C44&amp;" "&amp;D44&amp;" "&amp;E44</f>
+        <v xml:space="preserve"> Practitioner </v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="B45" t="str">
+        <f>C45&amp;" "&amp;D45&amp;" "&amp;E45</f>
+        <v xml:space="preserve">Senior Practitioner </v>
+      </c>
+      <c r="C45" t="s">
+        <v>366</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="17" t="s">
+        <v>414</v>
+      </c>
+      <c r="B46" t="str">
+        <f>C46&amp;" "&amp;D46&amp;" "&amp;E46</f>
+        <v xml:space="preserve"> Programmadirecteur </v>
+      </c>
+      <c r="D46" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="17" t="s">
+        <v>415</v>
+      </c>
+      <c r="B47" t="str">
+        <f>C47&amp;" "&amp;D47&amp;" "&amp;E47</f>
+        <v xml:space="preserve"> Programmamanager </v>
+      </c>
+      <c r="D47" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="17" t="s">
+        <v>416</v>
+      </c>
+      <c r="B48" t="str">
+        <f>C48&amp;" "&amp;D48&amp;" "&amp;E48</f>
+        <v xml:space="preserve"> Stagiair </v>
+      </c>
+      <c r="D48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="B49" t="str">
+        <f>C49&amp;" "&amp;D49&amp;" "&amp;E49</f>
+        <v xml:space="preserve"> Topmanager </v>
+      </c>
+      <c r="D49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A3:E51">
+    <sortCondition ref="D3:D51"/>
+    <sortCondition ref="E3:E51"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>